<commit_message>
Move task select condition into spreadsheet
Only select ACTIVE and INACTIVE tasks, and set the status field
to "Not started" for all selected tasks.
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F00D23-073E-AF4E-AD08-C89EB2157A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980BF31B-5EF6-4D44-9E30-47E8215B3BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="225">
   <si>
     <t>table_name</t>
   </si>
@@ -685,16 +685,19 @@
     <t>sup_activity</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
     <t>join</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Only transform tasks with ACTIVE and INACTIVE statuses, both of which get a value of 'Not started' for this field (set in the tasks.py transform)</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "Status", "values": ["ACTIVE", "INACTIVE"]}</t>
+  </si>
+  <si>
+    <t>Case, Status</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF42D79-4151-C94E-B150-CAB1CD330C33}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1091,7 +1094,7 @@
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="56.6640625" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1137,8 +1140,11 @@
       <c r="F2" t="s">
         <v>219</v>
       </c>
+      <c r="G2" t="s">
+        <v>223</v>
+      </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1152,7 +1158,7 @@
         <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1164,9 +1170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1360,18 +1366,14 @@
       <c r="E6" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="M6" s="7"/>
       <c r="P6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="Q6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="20" customFormat="1" ht="15">

</xml_diff>

<commit_message>
Default assignee should not be 1 for tasks
There is no assignee with an ID of 1, so set the default assignee
for tasks to 2 instead.
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980BF31B-5EF6-4D44-9E30-47E8215B3BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D859382-E031-214B-8855-E9F6B7883C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -1085,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF42D79-4151-C94E-B150-CAB1CD330C33}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1170,9 +1170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1300,7 +1300,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>24</v>
@@ -3020,7 +3020,9 @@
   </sheetPr>
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>